<commit_message>
feat(fixtures): add deterministic image-in-cell richData XLSX fixture
- Update fixtures/xlsx/generate_fixtures.py to generate an image-in-cell richData workbook with explicit Content_Types overrides (metadata + richValue parts), vm="0" cell, and rId99 metadata relationship\n- Regenerate fixtures/xlsx/basic/image-in-cell-richdata.xlsx deterministically (fixed ZIP timestamps, 1x1 PNG)\n- Add formula-xlsx test asserting the expected richData parts and wiring are present
</commit_message>
<xml_diff>
--- a/fixtures/xlsx/basic/image-in-cell-richdata.xlsx
+++ b/fixtures/xlsx/basic/image-in-cell-richdata.xlsx
@@ -8,10 +8,19 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="0" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" maxSupportedVersion="120000"/>
   </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3E2803F5-59A4-4A43-8C86-93BA0C219F4F}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <valueMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
@@ -65,7 +74,7 @@
 <file path=xl/richData/richValue.xml><?xml version="1.0" encoding="utf-8"?>
 <rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <rv s="0" t="image">
-    <v>0</v>
+    <v kind="rel">0</v>
   </rv>
 </rvData>
 </file>
@@ -77,8 +86,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetData>
     <row r="1">
       <c r="A1" vm="0">

</xml_diff>